<commit_message>
[improvements] - better "temp" directory creation strategy to reduce collisions over time. - code refactoring to reduce duplication.
[web]
- added additional configurations on chromedriver (for chrome browser) to ease security restriction for testing:
  - allow to run "insecure" (http) content locally
  - allow access to local files
  - allow for auth prompt when crossing site origin
  - enable input event handling by the window manager

Signed-off-by: automike <mike.liu@covetrus.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_config_expression.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_config_expression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12645" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2251,8 +2251,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -2311,14 +2311,50 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2328,7 +2364,46 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2343,75 +2418,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2419,9 +2426,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2434,17 +2441,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2476,7 +2476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2488,7 +2494,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2500,7 +2512,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2512,151 +2656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2703,19 +2703,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2737,8 +2726,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2747,8 +2738,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2769,6 +2760,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2783,24 +2789,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2818,128 +2818,128 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5680,16 +5680,16 @@
   <sheetPr/>
   <dimension ref="A1:O297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39.625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" customWidth="1"/>
     <col min="4" max="4" width="31.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="48.75" style="5" customWidth="1"/>
@@ -6046,7 +6046,7 @@
       <c r="N12" s="22"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" ht="24" customHeight="1" spans="1:15">
+    <row r="13" ht="90" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="24" t="s">
@@ -10971,10 +10971,10 @@
   <sheetPr/>
   <dimension ref="A1:O297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>

</xml_diff>